<commit_message>
some extra files with the terminal password encrypted as well.
</commit_message>
<xml_diff>
--- a/New Terminals/MILL-NewTerminals2021-Changes.xlsx
+++ b/New Terminals/MILL-NewTerminals2021-Changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5744CEEE-F8C3-4CBD-9CB7-29CA12241F08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EB08B6-0C83-4B5A-A779-9D825E9DAF52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0388F361-8B5F-46E5-9EBD-DCE0B56DC71F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
   <si>
     <t>Ficheiros Novos</t>
   </si>
@@ -344,6 +344,39 @@
   </si>
   <si>
     <t>ficheiro de linkagem do programa errlog que se inclui o novo ficheiro mesolm para associar na linkagem e ter acesso ao subroutine respectivo</t>
+  </si>
+  <si>
+    <t>page.for</t>
+  </si>
+  <si>
+    <t>VISION menu 4, listagem de telas existentes as quais foi adicionada uma nova tela chama olmsnp que chama uma subroutine OLMSNP</t>
+  </si>
+  <si>
+    <t>tstlog.for</t>
+  </si>
+  <si>
+    <t>programa utilitario para testar escrita e leitura das transações no tmf (não chega a escrever no tmf mas sim usa tralog e logbuf em que passa o buff directemante)</t>
+  </si>
+  <si>
+    <t>kilsys.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">script ou command procedure que serve para terminar abrutamente os processos relativos  ao sistema de Jogo Millennium </t>
+  </si>
+  <si>
+    <t>DMQ_OLM_CONFIG.COM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X</t>
+  </si>
+  <si>
+    <t>script ou command procedure que serve para alterar o ficheiro de configuração do MessageQ que DMQ.INI e alterar qual é maquina que primaria e qual é a failover</t>
+  </si>
+  <si>
+    <t>olmcommon.for</t>
+  </si>
+  <si>
+    <t>ficheiro de código fonte que contêm subroutines que servem para invocar RTL (Remove from The bottom of the List) e ABL (Add to the Bottom of the List) respectivamente.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +509,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>125365</xdr:colOff>
+      <xdr:colOff>122190</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>381461</xdr:rowOff>
     </xdr:to>
@@ -520,9 +553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>124173</xdr:colOff>
+      <xdr:colOff>120998</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>410511</xdr:rowOff>
+      <xdr:rowOff>407336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -564,9 +597,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>257929</xdr:colOff>
+      <xdr:colOff>254754</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>654580</xdr:rowOff>
+      <xdr:rowOff>657755</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -608,9 +641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>124270</xdr:colOff>
+      <xdr:colOff>121094</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>66931</xdr:rowOff>
+      <xdr:rowOff>63756</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -945,14 +978,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A849B54-E80B-432E-A0A3-476BEDB1F586}">
   <dimension ref="D3:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F49" sqref="F48:F49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1468,79 +1501,114 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>

</xml_diff>